<commit_message>
Refactor Stack class in Stack.js
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julih\Insync\jcc30986@gmail.com\drive\Sandbox\CoreJSExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DE3705-9291-4E9E-A7B5-878C81278F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90948E36-F744-40DF-81B1-F109721F5176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Exercise</t>
   </si>
@@ -42,7 +42,10 @@
     <t>BasicDataStructure</t>
   </si>
   <si>
-    <t>On progress</t>
+    <t>FoodOrderingSystem</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -98,8 +101,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1F8806F7-E7F6-42CC-9D5C-EE896386B282}" name="Exercise"/>
     <tableColumn id="2" xr3:uid="{6A1269B4-3521-49F8-B8A0-0C2F8ABDD160}" name="TypeScripted"/>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,10 +407,40 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor Warehouse class to use TypeScript and add Mediator support
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julih\Insync\jcc30986@gmail.com\drive\Sandbox\CoreJSExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90948E36-F744-40DF-81B1-F109721F5176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9446B985-E056-47D5-9AD4-BE9E3B0DE2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Exercise</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>FoodOrderingSystem</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
   </si>
 </sst>
 </file>
@@ -377,7 +374,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +412,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove unused code and files
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julih\Insync\jcc30986@gmail.com\drive\Sandbox\CoreJSExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D401F0-BBAB-4287-A54A-06B8244BE35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E3D00D-B029-4FCA-A6C0-6759265ADABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Exercise</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>RedBlackTree</t>
+  </si>
+  <si>
+    <t>Fractions</t>
+  </si>
+  <si>
+    <t>On progress</t>
   </si>
 </sst>
 </file>
@@ -104,8 +110,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B6" totalsRowShown="0">
-  <autoFilter ref="A1:B6" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1F8806F7-E7F6-42CC-9D5C-EE896386B282}" name="Exercise"/>
     <tableColumn id="2" xr3:uid="{6A1269B4-3521-49F8-B8A0-0C2F8ABDD160}" name="TypeScripted"/>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +438,17 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +464,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B6">
+  <conditionalFormatting sqref="B2:B7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Refactor Circle and Scene classes, and update index.html and script.js files
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julih\Insync\jcc30986@gmail.com\drive\Sandbox\CoreJSExercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E3D00D-B029-4FCA-A6C0-6759265ADABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95AD465B-F223-4FF5-8F34-78DD13C892C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Exercise</t>
   </si>
@@ -54,7 +54,7 @@
     <t>Fractions</t>
   </si>
   <si>
-    <t>On progress</t>
+    <t>Scene</t>
   </si>
 </sst>
 </file>
@@ -110,8 +110,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B7" totalsRowShown="0">
-  <autoFilter ref="A1:B7" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}" name="Table2" displayName="Table2" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8" xr:uid="{F02CF6C6-C442-41E3-971B-DF1B8BEFD105}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1F8806F7-E7F6-42CC-9D5C-EE896386B282}" name="Exercise"/>
     <tableColumn id="2" xr3:uid="{6A1269B4-3521-49F8-B8A0-0C2F8ABDD160}" name="TypeScripted"/>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,6 +448,11 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -464,7 +469,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B7">
+  <conditionalFormatting sqref="B2:B8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>